<commit_message>
Teste 1,2,3 passando com excel
</commit_message>
<xml_diff>
--- a/excel/ForwardCar.xlsx
+++ b/excel/ForwardCar.xlsx
@@ -1,16 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7F11714-9E8E-4DCF-88AA-A6C847BADBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B52991BC-E60C-405A-A5BF-47FF2FD084C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste1" sheetId="1" r:id="rId1"/>
-    <sheet name="Teste2" sheetId="2" r:id="rId2"/>
-    <sheet name="Teste3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -420,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,86 +471,18 @@
         <v>123456</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291C7DDD-73EB-456D-83F2-88ED9079B3C0}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>123456</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840393A9-629A-4D8C-856A-E5B4F97D8C0C}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>852456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Teste 1 ao 4 funcionando
</commit_message>
<xml_diff>
--- a/excel/ForwardCar.xlsx
+++ b/excel/ForwardCar.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B52991BC-E60C-405A-A5BF-47FF2FD084C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D990AABA-D248-43CF-BDDD-F8B97409FB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teste2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>firstname</t>
   </si>
@@ -67,6 +68,12 @@
   </si>
   <si>
     <t>zimmerf</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>modelo de carro</t>
   </si>
 </sst>
 </file>
@@ -418,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -485,6 +492,36 @@
         <v>123456</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE05F03-81D2-4BA1-8D2B-8064CB03D512}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
teste 1 funcionando com for
</commit_message>
<xml_diff>
--- a/excel/ForwardCar.xlsx
+++ b/excel/ForwardCar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D990AABA-D248-43CF-BDDD-F8B97409FB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{130E9E88-818E-44AF-8108-A4EBFB175709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>firstname</t>
   </si>
@@ -52,7 +52,7 @@
     <t>Zimmer</t>
   </si>
   <si>
-    <t>zimmer1</t>
+    <t>zimmer12</t>
   </si>
   <si>
     <t>Luciana</t>
@@ -61,19 +61,16 @@
     <t xml:space="preserve">Alves </t>
   </si>
   <si>
-    <t>morais1</t>
+    <t>morais12</t>
   </si>
   <si>
     <t>Fabiana</t>
   </si>
   <si>
-    <t>zimmerf</t>
+    <t>zimmerfer</t>
   </si>
   <si>
     <t>Acura</t>
-  </si>
-  <si>
-    <t>modelo de carro</t>
   </si>
 </sst>
 </file>
@@ -425,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,33 +489,23 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE05F03-81D2-4BA1-8D2B-8064CB03D512}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB24576-128D-4965-B42C-879C5C11488F}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
teste 1,2 e 3 ok
</commit_message>
<xml_diff>
--- a/excel/ForwardCar.xlsx
+++ b/excel/ForwardCar.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{130E9E88-818E-44AF-8108-A4EBFB175709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{425E4B09-5EB1-4975-B54D-1E8EF0EF042A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>firstname</t>
   </si>
@@ -70,7 +70,13 @@
     <t>zimmerfer</t>
   </si>
   <si>
-    <t>Acura</t>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zimmerf </t>
+  </si>
+  <si>
+    <t>Felipe</t>
   </si>
 </sst>
 </file>
@@ -424,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,17 +502,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB24576-128D-4965-B42C-879C5C11488F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>852456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>